<commit_message>
Product add (all type ended), product delete, manufacturer list, add, delete
</commit_message>
<xml_diff>
--- a/docs/data_structure.xlsx
+++ b/docs/data_structure.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\itshopping_back\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\git repositories\itshopping_back\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5904DB-7C8E-4AD6-B5BD-6242B10E4C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="데이터 구조 설계" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="749">
   <si>
     <t>CPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3024,12 +3025,412 @@
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>{
+    "prod": {
+        "pi_manufacturer_seq": 3,
+        "pi_name": "B450M AORUS ELITE",
+        "pi_price": "95000",
+        "pi_release_dt": "2019-12-01",
+        "pi_type": 3
+    },
+    "data": {
+        "detail_mb_socket": "AM4",
+        "detail_mb_dram_type": "DDR4",
+        "detail_mb_dram_spd": "3600",
+        "detail_mb_dram_slots": "4",
+        "detail_mb_form": "M-ATX",
+        "detail_mb_vertical": "244",
+        "detail_mb_horz": "244",
+        "detail_mb_pwr_phase": "4+3",
+        "detail_mb_hdmi": "1",
+        "detail_mb_dvi": "1",
+        "detail_mb_dsub": "0",
+        "detail_mb_dp": "0",
+        "detail_mb_wifi": "0",
+        "detail_mb_rj45": "1",
+        "detail_mb_pci_ver": "PCIe4.0x16",
+        "detail_mb_pci": "2",
+        "detail_mb_m2": "2",
+        "detail_mb_m2_type": "PCIe3.0x4",
+        "detail_mb_m2_size": "2280",
+        "detail_mb_sata_cnt": "6",
+        "detail_mb_usb20": "2",
+        "detail_mb_usb30": "0",
+        "detail_mb_usb31": "4",
+        "detail_mb_usb32": "2",
+        "detail_mb_usbc": "0",
+        "detail_mb_thunderbolt3": "0",
+        "detail_mb_thunderbolt4": "0",
+        "detail_mb_thunderbolt5": "0"
+    },
+    "img_list": [{
+            "prod_img_order": 1,
+            "prod_img_file": "dummy1.png",
+            "prod_img_thumbnail": 1
+        },
+        {
+            "prod_img_order": 2,
+            "prod_img_file": "dummy2.png",
+            "prod_img_thumbnail": 0
+        },
+        {
+            "prod_img_order": 3,
+            "prod_img_file": "dummy3.png",
+            "prod_img_thumbnail": 0
+        }
+    ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "prod": {
+        "pi_manufacturer_seq": 5,
+        "pi_name": "870 EVO 1TB",
+        "pi_price": "130000",
+        "pi_release_dt": "2021-01-01",
+        "pi_type": 4
+    },
+    "data": {
+        "detail_ssd_interface":"SATA3",
+        "detail_ssd_iops":"98000",
+        "detail_ssd_read_spd":"560",
+        "detail_ssd_write_spd":"530",
+        "detail_ssd_volume_size":"1000",
+        "detail_ssd_dram_size":"512",
+        "detail_ssd_density":"TLC"
+    },
+    "img_list": [{
+            "prod_img_order": 1,
+            "prod_img_file": "dummy1.png",
+            "prod_img_thumbnail": 1
+        },
+        {
+            "prod_img_order": 2,
+            "prod_img_file": "dummy2.png",
+            "prod_img_thumbnail": 0
+        },
+        {
+            "prod_img_order": 3,
+            "prod_img_file": "dummy3.png",
+            "prod_img_thumbnail": 0
+        }
+    ]
+}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "prod": {
+        "pi_manufacturer_seq": 7,
+        "pi_name": "Class II 풀체인지 700W 80PLUS BRONZE 230V EU",
+        "pi_price": "76000",
+        "pi_release_dt": "2021-04-01",
+        "pi_type": 6
+    },
+    "data": {
+        "detail_pwr_rated":"700",
+        "detail_pwr_cert_rate":"BRONZE",
+        "detail_pwr_cable_type":"케이블일체형",
+        "detail_pwr_type":"ATX"
+    },
+    "img_list": [{
+            "prod_img_order": 1,
+            "prod_img_file": "dummy1.png",
+            "prod_img_thumbnail": 1
+        },
+        {
+            "prod_img_order": 2,
+            "prod_img_file": "dummy2.png",
+            "prod_img_thumbnail": 0
+        },
+        {
+            "prod_img_order": 3,
+            "prod_img_file": "dummy3.png",
+            "prod_img_thumbnail": 0
+        }
+    ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "prod": {
+    "pi_manufacturer_seq": 10,
+    "pi_name": "BR-1300BT",
+    "pi_price": "86500",
+    "pi_release_dt": "2022-02-01",
+    "pi_type": 10
+  },
+  "data": {
+    "detail_spk_channel": "2.0",
+    "detail_spk_bluetooth": "v5.0",
+    "detail_spk_output": "16"
+  },
+  "img_list": [
+    {
+      "prod_img_order": 1,
+      "prod_img_file": "dummy1.png",
+      "prod_img_thumbnail": 1
+    },
+    {
+      "prod_img_order": 2,
+      "prod_img_file": "dummy2.png",
+      "prod_img_thumbnail": 0
+    },
+    {
+      "prod_img_order": 3,
+      "prod_img_file": "dummy3.png",
+      "prod_img_thumbnail": 0
+    }
+  ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "prod": {
+        "pi_manufacturer_seq": 9,
+        "pi_name": "MX Anywhere 3",
+        "pi_price": "93000",
+        "pi_release_dt": "2020-10-01",
+        "pi_type": 9
+    },
+    "data": {
+        "detail_mouse_sensor":"레이저",
+        "detail_mouse_conn_type":"전용동글",
+        "detail_mouse_dpi":"4000",
+        "detail_mouse_interface":"USB",
+        "detail_mouse_btns":"5"
+    },
+    "img_list": [{
+            "prod_img_order": 1,
+            "prod_img_file": "dummy1.png",
+            "prod_img_thumbnail": 1
+        },
+        {
+            "prod_img_order": 2,
+            "prod_img_file": "dummy2.png",
+            "prod_img_thumbnail": 0
+        },
+        {
+            "prod_img_order": 3,
+            "prod_img_file": "dummy3.png",
+            "prod_img_thumbnail": 0
+        }
+    ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "prod": {
+    "pi_manufacturer_seq": 9,
+    "pi_name": "G413 TKL SE",
+    "pi_price": "65000",
+    "pi_release_dt": "2022-02-01",
+    "pi_type": 8
+  },
+  "data": {
+    "detail_kbd_contact_type": "기계식",
+    "detail_kbd_conn_type": "유선",
+    "detail_kbd_shape": "텐키레스",
+    "detail_kbd_backlight": "단색",
+    "detail_kbd_interface": "USB",
+    "detail_kbd_key_cnt": "87"
+  },
+  "img_list": [
+    {
+      "prod_img_order": 1,
+      "prod_img_file": "dummy1.png",
+      "prod_img_thumbnail": 1
+    },
+    {
+      "prod_img_order": 2,
+      "prod_img_file": "dummy2.png",
+      "prod_img_thumbnail": 0
+    },
+    {
+      "prod_img_order": 3,
+      "prod_img_file": "dummy3.png",
+      "prod_img_thumbnail": 0
+    }
+  ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "prod": {
+    "pi_manufacturer_seq": 8,
+    "pi_name": "SUITMASTER P1000 강화유리",
+    "pi_price": "76000",
+    "pi_release_dt": "2021-03-01",
+    "pi_type": 7
+  },
+  "data": {
+    "detail_case_type": "미들타워",
+    "detail_case_board_type": "표준-ATX",
+    "detail_case_power_type": "ATX",
+    "detail_case_horz": "230",
+    "detail_case_vertical": "400",
+    "detail_case_height": "460",
+    "detail_case_usb20": "0",
+    "detail_case_usb30": "2",
+    "detail_case_usb31": "0",
+    "detail_case_usb32": "0",
+    "detail_case_usbc": "1",
+    "detail_case_mic": "1",
+    "detail_case_spk": "1"
+  },
+  "img_list": [
+    {
+      "prod_img_order": 1,
+      "prod_img_file": "dummy1.png",
+      "prod_img_thumbnail": 1
+    },
+    {
+      "prod_img_order": 2,
+      "prod_img_file": "dummy2.png",
+      "prod_img_thumbnail": 0
+    },
+    {
+      "prod_img_order": 3,
+      "prod_img_file": "dummy3.png",
+      "prod_img_thumbnail": 0
+    }
+  ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "prod": {
+    "pi_manufacturer_seq": 7,
+    "pi_name": "Class II 풀체인지 700W 80PLUS BRONZE 230V EU",
+    "pi_price": "76000",
+    "pi_release_dt": "2021-04-01",
+    "pi_type": 6
+  },
+  "data": {
+    "detail_pwr_rated": "700",
+    "detail_pwr_cert_rate": "BRONZE",
+    "detail_pwr_cable_type": "케이블일체형",
+    "detail_pwr_type": "ATX"
+  },
+  "img_list": [
+    {
+      "prod_img_order": 1,
+      "prod_img_file": "dummy1.png",
+      "prod_img_thumbnail": 1
+    },
+    {
+      "prod_img_order": 2,
+      "prod_img_file": "dummy2.png",
+      "prod_img_thumbnail": 0
+    },
+    {
+      "prod_img_order": 3,
+      "prod_img_file": "dummy3.png",
+      "prod_img_thumbnail": 0
+    }
+  ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "prod": {
+        "pi_manufacturer_seq": 6,
+        "pi_name": "BarraCuda 5400/256M",
+        "pi_price": "110000",
+        "pi_release_dt": "2017-11-01",
+        "pi_type": 5
+    },
+    "data": {
+        "detail_hdd_volume_size":"3000",
+        "detail_hdd_buffer_size":"256",
+        "detail_hdd_rpm":"5400",
+        "detail_hdd_read_spd":"190",
+        "detail_hdd_write_spd":"190"
+    },
+    "img_list": [{
+            "prod_img_order": 1,
+            "prod_img_file": "dummy1.png",
+            "prod_img_thumbnail": 1
+        },
+        {
+            "prod_img_order": 2,
+            "prod_img_file": "dummy2.png",
+            "prod_img_thumbnail": 0
+        },
+        {
+            "prod_img_order": 3,
+            "prod_img_file": "dummy3.png",
+            "prod_img_thumbnail": 0
+        }
+    ]
+}
+"detail_hdd_volume_size":"",
+"detail_hdd_buffer_size":"",
+"detail_hdd_rpm":"",
+"detail_hdd_read_spd":"",
+"detail_hdd_write_spd":"",
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M/B 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSD 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스피커 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키보드 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>케이스 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파워서플라이 정보 추가 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3055,6 +3456,14 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -3128,20 +3537,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3422,7 +3831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:W72"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -5489,11 +5898,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G302"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5511,11 +5920,11 @@
       <c r="B2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="4" t="s">
         <v>194</v>
       </c>
@@ -5831,11 +6240,11 @@
       <c r="B21" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="4" t="s">
         <v>194</v>
       </c>
@@ -5903,11 +6312,11 @@
       <c r="B26" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="4" t="s">
         <v>194</v>
       </c>
@@ -6155,11 +6564,11 @@
       <c r="B42" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
       <c r="F42" s="4" t="s">
         <v>194</v>
       </c>
@@ -6467,11 +6876,11 @@
       <c r="B62" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="4" t="s">
         <v>194</v>
       </c>
@@ -6973,11 +7382,11 @@
       <c r="B94" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
       <c r="F94" s="4" t="s">
         <v>194</v>
       </c>
@@ -7141,11 +7550,11 @@
       <c r="B105" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
       <c r="F105" s="4" t="s">
         <v>194</v>
       </c>
@@ -7277,11 +7686,11 @@
       <c r="B114" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="D114" s="9"/>
-      <c r="E114" s="9"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
       <c r="F114" s="4" t="s">
         <v>194</v>
       </c>
@@ -7397,11 +7806,11 @@
       <c r="B122" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="D122" s="9"/>
-      <c r="E122" s="9"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
       <c r="F122" s="4" t="s">
         <v>194</v>
       </c>
@@ -7661,11 +8070,11 @@
       <c r="B139" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C139" s="9" t="s">
+      <c r="C139" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="D139" s="9"/>
-      <c r="E139" s="9"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
       <c r="F139" s="4" t="s">
         <v>194</v>
       </c>
@@ -7813,11 +8222,11 @@
       <c r="B149" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C149" s="9" t="s">
+      <c r="C149" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="D149" s="9"/>
-      <c r="E149" s="9"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
       <c r="F149" s="4" t="s">
         <v>194</v>
       </c>
@@ -7949,11 +8358,11 @@
       <c r="B158" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C158" s="9" t="s">
+      <c r="C158" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="D158" s="9"/>
-      <c r="E158" s="9"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
       <c r="F158" s="4" t="s">
         <v>194</v>
       </c>
@@ -8053,11 +8462,11 @@
       <c r="B165" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C165" s="9" t="s">
+      <c r="C165" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="D165" s="9"/>
-      <c r="E165" s="9"/>
+      <c r="D165" s="7"/>
+      <c r="E165" s="7"/>
       <c r="F165" s="4" t="s">
         <v>194</v>
       </c>
@@ -8195,11 +8604,11 @@
       <c r="B174" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C174" s="9" t="s">
+      <c r="C174" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="D174" s="9"/>
-      <c r="E174" s="9"/>
+      <c r="D174" s="7"/>
+      <c r="E174" s="7"/>
       <c r="F174" s="4" t="s">
         <v>194</v>
       </c>
@@ -8449,11 +8858,11 @@
       <c r="B190" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C190" s="9" t="s">
+      <c r="C190" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="D190" s="9"/>
-      <c r="E190" s="9"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="7"/>
       <c r="F190" s="4" t="s">
         <v>194</v>
       </c>
@@ -8554,26 +8963,26 @@
       </c>
     </row>
     <row r="196" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="7"/>
-      <c r="C196" s="7"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7"/>
-      <c r="F196" s="7"/>
-      <c r="G196" s="7"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
     </row>
     <row r="197" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C197" s="9" t="s">
+      <c r="C197" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="D197" s="9"/>
-      <c r="E197" s="9"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="7"/>
       <c r="F197" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G197" s="5" t="s">
+      <c r="G197" s="3" t="s">
         <v>712</v>
       </c>
     </row>
@@ -8598,92 +9007,92 @@
       </c>
     </row>
     <row r="199" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="5" t="s">
+      <c r="B199" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="C199" s="5" t="s">
+      <c r="C199" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D199" s="5" t="s">
+      <c r="D199" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E199" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F199" s="5" t="s">
+      <c r="E199" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F199" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G199" s="5" t="s">
+      <c r="G199" s="3" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="200" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="5" t="s">
+      <c r="B200" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="C200" s="5" t="s">
+      <c r="C200" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D200" s="5" t="s">
+      <c r="D200" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="E200" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F200" s="5"/>
-      <c r="G200" s="5" t="s">
+      <c r="E200" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="201" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="5" t="s">
+      <c r="B201" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="C201" s="5" t="s">
+      <c r="C201" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="D201" s="5"/>
-      <c r="E201" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F201" s="5"/>
-      <c r="G201" s="5" t="s">
+      <c r="D201" s="3"/>
+      <c r="E201" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="202" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="5" t="s">
+      <c r="B202" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="C202" s="5" t="s">
+      <c r="C202" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="D202" s="5"/>
-      <c r="E202" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F202" s="5" t="s">
+      <c r="D202" s="3"/>
+      <c r="E202" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F202" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="G202" s="5" t="s">
+      <c r="G202" s="3" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="203" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="5" t="s">
+      <c r="B203" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="C203" s="5" t="s">
+      <c r="C203" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="D203" s="5"/>
-      <c r="E203" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F203" s="5">
+      <c r="D203" s="3"/>
+      <c r="E203" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F203" s="3">
         <v>1</v>
       </c>
-      <c r="G203" s="5" t="s">
+      <c r="G203" s="3" t="s">
         <v>725</v>
       </c>
     </row>
@@ -8691,11 +9100,11 @@
       <c r="B205" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C205" s="9" t="s">
+      <c r="C205" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="D205" s="9"/>
-      <c r="E205" s="9"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
       <c r="F205" s="4" t="s">
         <v>194</v>
       </c>
@@ -8801,11 +9210,11 @@
       <c r="B212" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C212" s="9" t="s">
+      <c r="C212" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D212" s="9"/>
-      <c r="E212" s="9"/>
+      <c r="D212" s="7"/>
+      <c r="E212" s="7"/>
       <c r="F212" s="4" t="s">
         <v>194</v>
       </c>
@@ -8965,11 +9374,11 @@
       <c r="B222" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C222" s="9" t="s">
+      <c r="C222" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="D222" s="9"/>
-      <c r="E222" s="9"/>
+      <c r="D222" s="7"/>
+      <c r="E222" s="7"/>
       <c r="F222" s="4" t="s">
         <v>194</v>
       </c>
@@ -9109,11 +9518,11 @@
       <c r="B231" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C231" s="9" t="s">
+      <c r="C231" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="D231" s="9"/>
-      <c r="E231" s="9"/>
+      <c r="D231" s="7"/>
+      <c r="E231" s="7"/>
       <c r="F231" s="4" t="s">
         <v>194</v>
       </c>
@@ -9233,11 +9642,11 @@
       <c r="B239" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C239" s="9" t="s">
+      <c r="C239" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="D239" s="9"/>
-      <c r="E239" s="9"/>
+      <c r="D239" s="7"/>
+      <c r="E239" s="7"/>
       <c r="F239" s="4" t="s">
         <v>194</v>
       </c>
@@ -9314,7 +9723,7 @@
       <c r="E243" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F243" s="6" t="s">
+      <c r="F243" s="5" t="s">
         <v>610</v>
       </c>
       <c r="G243" s="3" t="s">
@@ -9361,11 +9770,11 @@
       <c r="B247" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C247" s="9" t="s">
+      <c r="C247" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="D247" s="9"/>
-      <c r="E247" s="9"/>
+      <c r="D247" s="7"/>
+      <c r="E247" s="7"/>
       <c r="F247" s="4" t="s">
         <v>194</v>
       </c>
@@ -9444,7 +9853,7 @@
       <c r="E251" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F251" s="6"/>
+      <c r="F251" s="5"/>
       <c r="G251" s="3" t="s">
         <v>623</v>
       </c>
@@ -9471,11 +9880,11 @@
       <c r="B254" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C254" s="9" t="s">
+      <c r="C254" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="D254" s="9"/>
-      <c r="E254" s="9"/>
+      <c r="D254" s="7"/>
+      <c r="E254" s="7"/>
       <c r="F254" s="4" t="s">
         <v>194</v>
       </c>
@@ -9552,7 +9961,7 @@
       <c r="E258" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F258" s="6"/>
+      <c r="F258" s="5"/>
       <c r="G258" s="3" t="s">
         <v>633</v>
       </c>
@@ -9579,11 +9988,11 @@
       <c r="B261" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C261" s="9" t="s">
+      <c r="C261" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="D261" s="9"/>
-      <c r="E261" s="9"/>
+      <c r="D261" s="7"/>
+      <c r="E261" s="7"/>
       <c r="F261" s="4" t="s">
         <v>194</v>
       </c>
@@ -9660,7 +10069,7 @@
       <c r="E265" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F265" s="6"/>
+      <c r="F265" s="5"/>
       <c r="G265" s="3" t="s">
         <v>519</v>
       </c>
@@ -9694,7 +10103,7 @@
       <c r="E267" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F267" s="6">
+      <c r="F267" s="5">
         <v>1</v>
       </c>
       <c r="G267" s="3" t="s">
@@ -9728,7 +10137,7 @@
       <c r="E269" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F269" s="6"/>
+      <c r="F269" s="5"/>
       <c r="G269" s="3" t="s">
         <v>651</v>
       </c>
@@ -9760,7 +10169,7 @@
       <c r="E271" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F271" s="6"/>
+      <c r="F271" s="5"/>
       <c r="G271" s="3" t="s">
         <v>662</v>
       </c>
@@ -9776,7 +10185,7 @@
       <c r="E272" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F272" s="6"/>
+      <c r="F272" s="5"/>
       <c r="G272" s="3" t="s">
         <v>658</v>
       </c>
@@ -9808,7 +10217,7 @@
       <c r="E274" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F274" s="6"/>
+      <c r="F274" s="5"/>
       <c r="G274" s="3" t="s">
         <v>660</v>
       </c>
@@ -9840,7 +10249,7 @@
       <c r="E276" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F276" s="6"/>
+      <c r="F276" s="5"/>
       <c r="G276" s="3" t="s">
         <v>666</v>
       </c>
@@ -9913,11 +10322,11 @@
       <c r="B282" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C282" s="9" t="s">
+      <c r="C282" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="D282" s="9"/>
-      <c r="E282" s="9"/>
+      <c r="D282" s="7"/>
+      <c r="E282" s="7"/>
       <c r="F282" s="4" t="s">
         <v>194</v>
       </c>
@@ -9996,7 +10405,7 @@
       <c r="E286" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F286" s="6"/>
+      <c r="F286" s="5"/>
       <c r="G286" s="3" t="s">
         <v>684</v>
       </c>
@@ -10030,7 +10439,7 @@
       <c r="E288" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F288" s="6"/>
+      <c r="F288" s="5"/>
       <c r="G288" s="3" t="s">
         <v>687</v>
       </c>
@@ -10039,11 +10448,11 @@
       <c r="B290" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C290" s="9" t="s">
+      <c r="C290" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="D290" s="9"/>
-      <c r="E290" s="9"/>
+      <c r="D290" s="7"/>
+      <c r="E290" s="7"/>
       <c r="F290" s="4" t="s">
         <v>194</v>
       </c>
@@ -10120,7 +10529,7 @@
       <c r="E294" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F294" s="6"/>
+      <c r="F294" s="5"/>
       <c r="G294" s="3" t="s">
         <v>694</v>
       </c>
@@ -10154,7 +10563,7 @@
       <c r="E296" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F296" s="6" t="s">
+      <c r="F296" s="5" t="s">
         <v>514</v>
       </c>
       <c r="G296" s="3" t="s">
@@ -10172,7 +10581,7 @@
       <c r="E297" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F297" s="6"/>
+      <c r="F297" s="5"/>
       <c r="G297" s="3" t="s">
         <v>700</v>
       </c>
@@ -10181,11 +10590,11 @@
       <c r="B299" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C299" s="9" t="s">
+      <c r="C299" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="D299" s="9"/>
-      <c r="E299" s="9"/>
+      <c r="D299" s="7"/>
+      <c r="E299" s="7"/>
       <c r="F299" s="4" t="s">
         <v>194</v>
       </c>
@@ -10253,11 +10662,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C282:E282"/>
+    <mergeCell ref="C290:E290"/>
+    <mergeCell ref="C299:E299"/>
+    <mergeCell ref="C222:E222"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C247:E247"/>
+    <mergeCell ref="C254:E254"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C261:E261"/>
     <mergeCell ref="C149:E149"/>
     <mergeCell ref="C158:E158"/>
     <mergeCell ref="C165:E165"/>
@@ -10267,19 +10684,11 @@
     <mergeCell ref="C114:E114"/>
     <mergeCell ref="C122:E122"/>
     <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C261:E261"/>
-    <mergeCell ref="C282:E282"/>
-    <mergeCell ref="C290:E290"/>
-    <mergeCell ref="C299:E299"/>
-    <mergeCell ref="C222:E222"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C247:E247"/>
-    <mergeCell ref="C254:E254"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C62:E62"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10288,31 +10697,133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="84.5" customWidth="1"/>
+    <col min="1" max="1" width="9" style="8"/>
+    <col min="2" max="2" width="84.5" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="349.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>728</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>